<commit_message>
Commit:"invoice-python" is stable; Rest:Unfinished
</commit_message>
<xml_diff>
--- a/Invoice/sale.xlsx
+++ b/Invoice/sale.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="25">
   <si>
     <t>Size</t>
   </si>
@@ -77,6 +77,18 @@
   </si>
   <si>
     <t>b7</t>
+  </si>
+  <si>
+    <t>GRADE</t>
+  </si>
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>c3</t>
   </si>
 </sst>
 </file>
@@ -898,242 +910,305 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B4" sqref="B4:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>13</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>1500</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>15</v>
       </c>
       <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>400</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
         <v>7</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>1100</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
         <v>3</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>17</v>
       </c>
       <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
         <v>5</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>2100</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>18</v>
       </c>
       <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
         <v>4</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>9000</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>19</v>
       </c>
       <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
         <v>8</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>1500</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>19</v>
       </c>
       <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
         <v>9</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>1500</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>19</v>
       </c>
       <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
         <v>6</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>2200</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
         <v>2</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>1400</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
         <v>10</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>250</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
         <v>11</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
         <v>7</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>700</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
         <v>12</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>100</v>
       </c>
     </row>

</xml_diff>